<commit_message>
JCA-Updated_Business_List 04102016 -Updated the business list spreadsheet function
</commit_message>
<xml_diff>
--- a/public/files/FeatherQ Weekly Numbers (3).xlsx
+++ b/public/files/FeatherQ Weekly Numbers (3).xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16729"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -35,13 +35,13 @@
     <t>number</t>
   </si>
   <si>
-    <t>jonas</t>
-  </si>
-  <si>
     <t>cebu city</t>
   </si>
   <si>
-    <t>cant</t>
+    <t xml:space="preserve">jonas </t>
+  </si>
+  <si>
+    <t>Cant reDd</t>
   </si>
 </sst>
 </file>
@@ -396,7 +396,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -414,10 +414,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
         <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
       </c>
       <c r="C2">
         <v>1231231</v>
@@ -428,7 +428,7 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C3">
         <v>23323</v>

</xml_diff>